<commit_message>
Finished special attacks, just need to insert them
</commit_message>
<xml_diff>
--- a/Files As of 6-2/SpecialAttacks.xlsx
+++ b/Files As of 6-2/SpecialAttacks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sierra\Documents\Post Bacc College Stuff\CSCD 349\Team Project\Current Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacob\Documents\GitHub\CSCD349_TeamProject\Files As of 6-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
   <si>
     <t>Good Guys</t>
   </si>
@@ -150,6 +150,21 @@
   </si>
   <si>
     <t>Roulette Heal</t>
+  </si>
+  <si>
+    <t>RapidShot</t>
+  </si>
+  <si>
+    <t>SummonWolf</t>
+  </si>
+  <si>
+    <t>SummonSkeleton</t>
+  </si>
+  <si>
+    <t>WhirlWindOfDeath</t>
+  </si>
+  <si>
+    <t>AvadaKedavra</t>
   </si>
 </sst>
 </file>
@@ -478,8 +493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +539,12 @@
       <c r="C2" t="s">
         <v>37</v>
       </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -558,6 +579,12 @@
       <c r="C4" t="s">
         <v>37</v>
       </c>
+      <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -592,6 +619,12 @@
       <c r="C6" t="s">
         <v>37</v>
       </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -623,6 +656,12 @@
       <c r="C8" t="s">
         <v>37</v>
       </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -632,6 +671,12 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>